<commit_message>
add DPYD plus CPIC-oncology drug assocs
</commit_message>
<xml_diff>
--- a/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
+++ b/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__geneOncoX/geneOncoX/data-raw/predisposition/curated_genes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__geneOncoX/geneOncoX/data-raw/predisposition/curated_genes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DF00B5-F543-3C42-8931-BCBDC826AC17}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13441C03-DC3F-EC47-8C4E-CAFB3D81D100}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29460" yWindow="6960" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{07135CED-1AF9-D746-918F-E5939A6BCAC3}"/>
+    <workbookView xWindow="8200" yWindow="5460" windowWidth="27640" windowHeight="16940" xr2:uid="{07135CED-1AF9-D746-918F-E5939A6BCAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="383">
   <si>
     <t>symbol</t>
   </si>
@@ -1169,6 +1169,12 @@
   </si>
   <si>
     <t>EGLN2</t>
+  </si>
+  <si>
+    <t>DPYD</t>
+  </si>
+  <si>
+    <t>ENSG00000188641</t>
   </si>
 </sst>
 </file>
@@ -1259,11 +1265,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1579,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DBA8AF-A017-894C-91C6-4A329FB0EFF2}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2774,6 +2781,14 @@
         <v>220</v>
       </c>
     </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B103" t="s">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2784,8 +2799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B058A35-2EA3-BA47-A9B9-67D9A55587CD}">
   <dimension ref="A1:A156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update curated cancer predisposition genes
</commit_message>
<xml_diff>
--- a/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
+++ b/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__geneOncoX/geneOncoX/data-raw/predisposition/curated_genes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13441C03-DC3F-EC47-8C4E-CAFB3D81D100}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126B6222-AC40-0C4E-9BD3-CEE5C9827E50}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="5460" windowWidth="27640" windowHeight="16940" xr2:uid="{07135CED-1AF9-D746-918F-E5939A6BCAC3}"/>
+    <workbookView xWindow="6580" yWindow="3900" windowWidth="27640" windowHeight="16940" xr2:uid="{07135CED-1AF9-D746-918F-E5939A6BCAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="385">
   <si>
     <t>symbol</t>
   </si>
@@ -1175,13 +1175,19 @@
   </si>
   <si>
     <t>ENSG00000188641</t>
+  </si>
+  <si>
+    <t>TTC7A</t>
+  </si>
+  <si>
+    <t>ENSG00000068724</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1207,6 +1213,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF666666"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1265,12 +1285,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1586,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DBA8AF-A017-894C-91C6-4A329FB0EFF2}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2787,6 +2809,14 @@
       </c>
       <c r="B103" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added mor CPG genes
</commit_message>
<xml_diff>
--- a/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
+++ b/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__geneOncoX/geneOncoX/data-raw/predisposition/curated_genes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12EF6FB-748B-724B-80AB-F8033ED231A4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7E2413-00A6-3849-B699-9D718FC95983}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="3900" windowWidth="27640" windowHeight="16940" xr2:uid="{07135CED-1AF9-D746-918F-E5939A6BCAC3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="402">
   <si>
     <t>symbol</t>
   </si>
@@ -1211,6 +1211,27 @@
   </si>
   <si>
     <t>PMID: 38143269</t>
+  </si>
+  <si>
+    <t>CHD1L</t>
+  </si>
+  <si>
+    <t>MYO3A</t>
+  </si>
+  <si>
+    <t>MYO5B</t>
+  </si>
+  <si>
+    <t>ENSG00000095777</t>
+  </si>
+  <si>
+    <t>ENSG00000167306</t>
+  </si>
+  <si>
+    <t>ENSG00000131778</t>
+  </si>
+  <si>
+    <t>PMID: 39037077</t>
   </si>
 </sst>
 </file>
@@ -1637,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DBA8AF-A017-894C-91C6-4A329FB0EFF2}">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2890,6 +2911,39 @@
       </c>
       <c r="D108" s="6" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>400</v>
+      </c>
+      <c r="B109" t="s">
+        <v>395</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>398</v>
+      </c>
+      <c r="B110" t="s">
+        <v>396</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>399</v>
+      </c>
+      <c r="B111" t="s">
+        <v>397</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added SAMHD1 and FAM111A
</commit_message>
<xml_diff>
--- a/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
+++ b/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__geneOncoX/geneOncoX/data-raw/predisposition/curated_genes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7E2413-00A6-3849-B699-9D718FC95983}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D546DD-1202-6643-B8ED-6DDC7FD70C5F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="3900" windowWidth="27640" windowHeight="16940" xr2:uid="{07135CED-1AF9-D746-918F-E5939A6BCAC3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="406">
   <si>
     <t>symbol</t>
   </si>
@@ -1232,6 +1232,18 @@
   </si>
   <si>
     <t>PMID: 39037077</t>
+  </si>
+  <si>
+    <t>FAM111A</t>
+  </si>
+  <si>
+    <t>SAMHD1</t>
+  </si>
+  <si>
+    <t>ENSG00000101347</t>
+  </si>
+  <si>
+    <t>ENSG00000166801</t>
   </si>
 </sst>
 </file>
@@ -1658,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DBA8AF-A017-894C-91C6-4A329FB0EFF2}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2944,6 +2956,22 @@
       </c>
       <c r="D111" s="6" t="s">
         <v>401</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>405</v>
+      </c>
+      <c r="B112" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>404</v>
+      </c>
+      <c r="B113" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding CDK12 as curated gene, dbNSFP updated to 5.3
</commit_message>
<xml_diff>
--- a/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
+++ b/data-raw/predisposition/curated_genes/predisposition_curated_other.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__geneOncoX/geneOncoX/data-raw/predisposition/curated_genes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D546DD-1202-6643-B8ED-6DDC7FD70C5F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD8A610-1A52-7440-A4FD-B8028023F330}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="3900" windowWidth="27640" windowHeight="16940" xr2:uid="{07135CED-1AF9-D746-918F-E5939A6BCAC3}"/>
+    <workbookView xWindow="8200" yWindow="3900" windowWidth="33440" windowHeight="18940" xr2:uid="{07135CED-1AF9-D746-918F-E5939A6BCAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="409">
   <si>
     <t>symbol</t>
   </si>
@@ -1244,6 +1244,15 @@
   </si>
   <si>
     <t>ENSG00000166801</t>
+  </si>
+  <si>
+    <t>CDK12</t>
+  </si>
+  <si>
+    <t>PMID:30333958</t>
+  </si>
+  <si>
+    <t>ENSG00000167258</t>
   </si>
 </sst>
 </file>
@@ -1670,10 +1679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DBA8AF-A017-894C-91C6-4A329FB0EFF2}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2966,12 +2975,23 @@
         <v>402</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>404</v>
       </c>
       <c r="B113" t="s">
         <v>403</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B114" t="s">
+        <v>406</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>